<commit_message>
Add primer V16S-U to list
</commit_message>
<xml_diff>
--- a/Project_clone/Report/primer_data.xlsx
+++ b/Project_clone/Report/primer_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
   <si>
     <t xml:space="preserve">Typ av analys</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t xml:space="preserve">AGGTCGTAAACCCCCTCGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V16S_U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACGAGAAGACCCYRYGRARCTT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCTHRRRANAGGATTGCGCTGTTA</t>
   </si>
   <si>
     <t xml:space="preserve">Art</t>
@@ -484,7 +493,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -715,7 +724,18 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3"/>
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -747,30 +767,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -778,13 +798,13 @@
         <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,13 +812,13 @@
         <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -832,162 +852,162 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,7 +1015,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,71 +1023,71 @@
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added vertebrate primer reference
</commit_message>
<xml_diff>
--- a/Project_clone/Report/primer_data.xlsx
+++ b/Project_clone/Report/primer_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t xml:space="preserve">Typ av analys</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">V16S_U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wang et al. 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Groddjur</t>
@@ -426,8 +429,8 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -688,25 +691,28 @@
       <c r="F14" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>55</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>